<commit_message>
copy old investment folder
</commit_message>
<xml_diff>
--- a/投资.xlsx
+++ b/投资.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Roy/Documents/Investment/Investment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Roy/Documents/Investment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F14F873-F612-6B47-B0B3-9C78564303C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0112081-3899-374E-9BD4-FE08D5FA827A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16600" activeTab="2" xr2:uid="{AC92DC69-0ADF-DF4F-ABE7-F2CC23157859}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16580" activeTab="2" xr2:uid="{AC92DC69-0ADF-DF4F-ABE7-F2CC23157859}"/>
   </bookViews>
   <sheets>
     <sheet name="基金" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
   <si>
     <t>东方红信用债</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>收益率</t>
+  </si>
+  <si>
+    <t>交银新生活力灵活配置混合</t>
+  </si>
+  <si>
+    <t>中银珍利混合C</t>
+  </si>
+  <si>
+    <t>长信乐信灵活配置混合C</t>
+  </si>
+  <si>
+    <t>广发趋势优选灵活配置混合A</t>
   </si>
 </sst>
 </file>
@@ -219,12 +231,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -774,7 +787,7 @@
       </c>
       <c r="I2" s="1">
         <f ca="1">NOW()</f>
-        <v>43962.636274652781</v>
+        <v>44001.715214351854</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -832,7 +845,7 @@
       </c>
       <c r="F5">
         <f ca="1">E5/B5 * 360 /($I$2-C5) * 100</f>
-        <v>3.2421902191629917</v>
+        <v>2.8166111759708845</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -850,7 +863,7 @@
       </c>
       <c r="F6">
         <f ca="1">E6/B6 * 360 /($I$2-C6) * 100</f>
-        <v>4.1996191827465168</v>
+        <v>3.6000300616585901</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -868,7 +881,7 @@
       </c>
       <c r="F9">
         <f ca="1">E9/B9 * 360 /($I$2-C9) * 100</f>
-        <v>2.59927182873151</v>
+        <v>1.9750106773627807</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -980,14 +993,15 @@
   <dimension ref="A1:AD28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="9" max="9" width="22.1640625" customWidth="1"/>
-    <col min="17" max="17" width="16.5" customWidth="1"/>
+    <col min="17" max="17" width="24.83203125" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -997,21 +1011,21 @@
       </c>
       <c r="B1">
         <f>G6+O6+W6+AD6</f>
-        <v>41443.769999999997</v>
+        <v>74332.63</v>
       </c>
       <c r="D1" t="s">
         <v>43</v>
       </c>
       <c r="E1">
         <f>O7+W7+AD7</f>
-        <v>1138991.6600000001</v>
+        <v>1182592.7</v>
       </c>
       <c r="G1" t="s">
         <v>44</v>
       </c>
       <c r="H1" s="3">
         <f>B1/E1</f>
-        <v>3.6386368272441953E-2</v>
+        <v>6.2855647595321709E-2</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
@@ -1045,7 +1059,7 @@
       </c>
       <c r="G6">
         <f>SUM(D:D)</f>
-        <v>23570.03</v>
+        <v>27614.989999999994</v>
       </c>
       <c r="I6" t="s">
         <v>30</v>
@@ -1060,12 +1074,15 @@
         <f>K6-J6 - 443.35*2</f>
         <v>4875.329999999999</v>
       </c>
+      <c r="M6">
+        <v>8443.75</v>
+      </c>
       <c r="N6" t="s">
         <v>29</v>
       </c>
       <c r="O6">
-        <f>SUM(L:L)</f>
-        <v>16824.09</v>
+        <f>SUM(L:L) +M6</f>
+        <v>25267.84</v>
       </c>
       <c r="Q6" t="s">
         <v>37</v>
@@ -1073,12 +1090,17 @@
       <c r="R6">
         <v>49000</v>
       </c>
+      <c r="T6">
+        <v>6079.31</v>
+      </c>
+      <c r="U6">
+        <v>9596.65</v>
+      </c>
       <c r="V6" t="s">
         <v>29</v>
       </c>
       <c r="W6">
-        <f>SUM(T:T)</f>
-        <v>-76.39</v>
+        <v>19046.560000000001</v>
       </c>
       <c r="Y6" t="s">
         <v>40</v>
@@ -1087,14 +1109,13 @@
         <v>110000</v>
       </c>
       <c r="AA6">
-        <v>407.31</v>
+        <v>735.78</v>
       </c>
       <c r="AC6" t="s">
         <v>29</v>
       </c>
       <c r="AD6">
-        <f>SUM(AA:AA)</f>
-        <v>1126.04</v>
+        <v>2403.2399999999998</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
@@ -1130,7 +1151,8 @@
         <v>43</v>
       </c>
       <c r="O7">
-        <v>818991.66</v>
+        <f>813077.18-143160.54</f>
+        <v>669916.64</v>
       </c>
       <c r="Q7" t="s">
         <v>38</v>
@@ -1138,30 +1160,37 @@
       <c r="R7">
         <v>30000</v>
       </c>
-      <c r="T7">
+      <c r="S7">
         <f>-22.47*2</f>
         <v>-44.94</v>
       </c>
+      <c r="T7">
+        <v>2750.68</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ref="U7:U8" si="0">T7+S7</f>
+        <v>2705.74</v>
+      </c>
       <c r="V7" t="s">
         <v>43</v>
       </c>
       <c r="W7">
-        <v>100000</v>
+        <v>201676.06</v>
       </c>
       <c r="Y7" t="s">
         <v>41</v>
       </c>
       <c r="Z7">
-        <v>50000</v>
+        <v>141000</v>
       </c>
       <c r="AA7">
-        <v>238.89</v>
+        <v>480.06</v>
       </c>
       <c r="AC7" t="s">
         <v>43</v>
       </c>
       <c r="AD7">
-        <v>220000</v>
+        <v>311000</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
@@ -1196,10 +1225,17 @@
       <c r="R8">
         <v>21000</v>
       </c>
-      <c r="T8">
+      <c r="S8">
         <f>-31.45</f>
         <v>-31.45</v>
       </c>
+      <c r="T8">
+        <v>2054.7199999999998</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>2023.2699999999998</v>
+      </c>
       <c r="Y8" t="s">
         <v>42</v>
       </c>
@@ -1207,7 +1243,7 @@
         <v>60000</v>
       </c>
       <c r="AA8">
-        <v>479.84</v>
+        <v>651.66999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
@@ -1237,6 +1273,23 @@
         <f>-443.35 + K9 - J9</f>
         <v>8886.11</v>
       </c>
+      <c r="Q9" t="s">
+        <v>45</v>
+      </c>
+      <c r="R9">
+        <v>27266.98</v>
+      </c>
+      <c r="S9">
+        <f>-18.37-30</f>
+        <v>-48.370000000000005</v>
+      </c>
+      <c r="T9">
+        <v>2.6</v>
+      </c>
+      <c r="U9">
+        <f>T9+S9</f>
+        <v>-45.77</v>
+      </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1261,6 +1314,19 @@
         <f>1630.96 + 1215.81</f>
         <v>2846.77</v>
       </c>
+      <c r="Q10" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10">
+        <v>18879.490000000002</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <f t="shared" ref="U10:U12" si="1">T10+S10</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1289,6 +1355,19 @@
         <f>-158.73</f>
         <v>-158.72999999999999</v>
       </c>
+      <c r="Q11" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11">
+        <v>11326.75</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1317,6 +1396,20 @@
         <f>-238.1</f>
         <v>-238.1</v>
       </c>
+      <c r="Q12" t="s">
+        <v>48</v>
+      </c>
+      <c r="R12">
+        <v>7544.21</v>
+      </c>
+      <c r="S12" s="5">
+        <f>-R12*0.15/100</f>
+        <v>-11.316314999999999</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="1"/>
+        <v>-11.316314999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1435,6 +1528,48 @@
         <v>1994.6</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>43971</v>
+      </c>
+      <c r="C19">
+        <v>50000</v>
+      </c>
+      <c r="D19">
+        <v>345.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2">
+        <v>43976</v>
+      </c>
+      <c r="C20">
+        <v>90000</v>
+      </c>
+      <c r="D20">
+        <v>845.55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2">
+        <v>44001</v>
+      </c>
+      <c r="C21">
+        <v>160000</v>
+      </c>
+      <c r="D21">
+        <v>1049.44</v>
+      </c>
+    </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
@@ -1443,7 +1578,7 @@
         <v>200000</v>
       </c>
       <c r="D26">
-        <v>5474.35</v>
+        <v>6889.49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1454,7 +1589,7 @@
         <v>56000</v>
       </c>
       <c r="D27">
-        <v>682.66</v>
+        <v>876.18</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1465,7 +1600,7 @@
         <v>50000</v>
       </c>
       <c r="D28">
-        <v>1296.73</v>
+        <v>1492.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>